<commit_message>
add table body builder.
</commit_message>
<xml_diff>
--- a/complianceReport.xlsx
+++ b/complianceReport.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>New York CPA</t>
   </si>
@@ -22,32 +19,94 @@
     <t>Page 1</t>
   </si>
   <si>
-    <t>Evan Hiner</t>
-  </si>
-  <si>
-    <t>License #: 123123123</t>
-  </si>
-  <si>
-    <t>Issue Date: 12/31/2017</t>
-  </si>
-  <si>
-    <t>Reporting Period: 12/30/2016 - 12/31/2017</t>
-  </si>
-  <si>
-    <t>Cycle Total: 12/30/2016 - 12/31/2017</t>
+    <t>Hiner, Evan</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">License #: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>123123123</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Issue Date: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>12/31/2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Reporting Period: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>12/30/2016 - 12/31/2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Cycle Total: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>12/30/2016 - 12/31/2017</t>
+    </r>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>SPONSOR</t>
+  </si>
+  <si>
+    <t>DELIVERY METHOD</t>
+  </si>
+  <si>
+    <t>GENERAL</t>
+  </si>
+  <si>
+    <t>ETHICS STATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,8 +129,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,132 +482,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:J8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="J1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="L2" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="I4" t="s">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="I5" t="s">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="I6" t="s">
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A2:D3"/>
-    <mergeCell ref="A4:F6"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="A7:D8"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="A3:F5"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="A6:D7"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add table cert data.
</commit_message>
<xml_diff>
--- a/complianceReport.xlsx
+++ b/complianceReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>New York CPA</t>
   </si>
@@ -82,10 +82,97 @@
     <t>DELIVERY METHOD</t>
   </si>
   <si>
-    <t>GENERAL</t>
-  </si>
-  <si>
     <t>ETHICS STATE</t>
+  </si>
+  <si>
+    <t>HOURS</t>
+  </si>
+  <si>
+    <t>2017-11-29T18:11:00.689Z</t>
+  </si>
+  <si>
+    <t>Preparing for 2018 Tax Updates (Group-Live)</t>
+  </si>
+  <si>
+    <t>BowmanKnopp</t>
+  </si>
+  <si>
+    <t>Live Course</t>
+  </si>
+  <si>
+    <t>2017-09-17T19:00:18.708Z</t>
+  </si>
+  <si>
+    <t>Demo In-House Course</t>
+  </si>
+  <si>
+    <t>Evan Hiner</t>
+  </si>
+  <si>
+    <t>2017-11-17T18:00:25.266Z</t>
+  </si>
+  <si>
+    <t>ASC 606 Update Training</t>
+  </si>
+  <si>
+    <t>2017-10-09T07:00:00.000Z</t>
+  </si>
+  <si>
+    <t>Group External Event</t>
+  </si>
+  <si>
+    <t>Group-Internet / Webinar</t>
+  </si>
+  <si>
+    <t>2017-11-15T20:00:58.198Z</t>
+  </si>
+  <si>
+    <t>Tax Updates November 2017</t>
+  </si>
+  <si>
+    <t>2017-08-01T21:00:07.085Z</t>
+  </si>
+  <si>
+    <t>Demo Course</t>
+  </si>
+  <si>
+    <t>2017-09-01T19:00:00.000Z</t>
+  </si>
+  <si>
+    <t>Fraud in the Digital Age</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>2017-12-18T18:30:00.000Z</t>
+  </si>
+  <si>
+    <t>Prolaera</t>
+  </si>
+  <si>
+    <t>2017-02-12T08:00:00.000Z</t>
+  </si>
+  <si>
+    <t>A&amp;A Conference 2017</t>
+  </si>
+  <si>
+    <t>WSCPA</t>
+  </si>
+  <si>
+    <t>Group-Live</t>
+  </si>
+  <si>
+    <t>2017-06-14T19:00:00.000Z</t>
+  </si>
+  <si>
+    <t>Federal Tax Updates</t>
+  </si>
+  <si>
+    <t>2017-09-01T07:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2017-11-01T08:00:00.000Z</t>
   </si>
 </sst>
 </file>
@@ -482,7 +569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J21"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -560,7 +647,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -573,21 +660,343 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
+      <c r="I8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
+      <c r="J8" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="16">
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="A3:F5"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="A6:D7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
fix table header and table row inputs.
</commit_message>
<xml_diff>
--- a/complianceReport.xlsx
+++ b/complianceReport.xlsx
@@ -654,10 +654,10 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="I8" t="s">
@@ -686,20 +686,14 @@
       <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>16</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
       <c r="I10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J10">
         <v>3</v>
@@ -712,20 +706,11 @@
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>16</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
       </c>
       <c r="J11">
         <v>1.5</v>
@@ -738,17 +723,8 @@
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>16</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
       </c>
       <c r="J12">
         <v>2</v>
@@ -761,17 +737,8 @@
       <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>24</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -784,20 +751,11 @@
       <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>19</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>16</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -810,20 +768,11 @@
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>16</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
       </c>
       <c r="J15">
         <v>4</v>
@@ -836,20 +785,11 @@
       <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>19</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>31</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
       </c>
       <c r="J16">
         <v>3</v>
@@ -862,20 +802,11 @@
       <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>33</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>16</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
       </c>
       <c r="J17">
         <v>2</v>
@@ -888,20 +819,11 @@
       <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>36</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>37</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
       </c>
       <c r="J18">
         <v>16</v>
@@ -914,20 +836,11 @@
       <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>19</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>16</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
       </c>
       <c r="J19">
         <v>2</v>
@@ -940,17 +853,8 @@
       <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>31</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
       </c>
       <c r="J20">
         <v>3</v>
@@ -963,17 +867,8 @@
       <c r="B21" t="s">
         <v>28</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>24</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
       </c>
       <c r="J21">
         <v>2</v>

</xml_diff>

<commit_message>
finish excel output data, preparing to refactor and modularize project.
</commit_message>
<xml_diff>
--- a/complianceReport.xlsx
+++ b/complianceReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>New York CPA</t>
   </si>
@@ -82,13 +82,13 @@
     <t>DELIVERY METHOD</t>
   </si>
   <si>
+    <t>HOURS</t>
+  </si>
+  <si>
     <t>ETHICS STATE</t>
   </si>
   <si>
-    <t>HOURS</t>
-  </si>
-  <si>
-    <t>2017-11-29T18:11:00.689Z</t>
+    <t>11/29/2017</t>
   </si>
   <si>
     <t>Preparing for 2018 Tax Updates (Group-Live)</t>
@@ -100,7 +100,7 @@
     <t>Live Course</t>
   </si>
   <si>
-    <t>2017-09-17T19:00:18.708Z</t>
+    <t>9/17/2017</t>
   </si>
   <si>
     <t>Demo In-House Course</t>
@@ -109,13 +109,13 @@
     <t>Evan Hiner</t>
   </si>
   <si>
-    <t>2017-11-17T18:00:25.266Z</t>
+    <t>11/17/2017</t>
   </si>
   <si>
     <t>ASC 606 Update Training</t>
   </si>
   <si>
-    <t>2017-10-09T07:00:00.000Z</t>
+    <t>10/9/2017</t>
   </si>
   <si>
     <t>Group External Event</t>
@@ -124,19 +124,19 @@
     <t>Group-Internet / Webinar</t>
   </si>
   <si>
-    <t>2017-11-15T20:00:58.198Z</t>
+    <t>11/15/2017</t>
   </si>
   <si>
     <t>Tax Updates November 2017</t>
   </si>
   <si>
-    <t>2017-08-01T21:00:07.085Z</t>
+    <t>8/1/2017</t>
   </si>
   <si>
     <t>Demo Course</t>
   </si>
   <si>
-    <t>2017-09-01T19:00:00.000Z</t>
+    <t>9/1/2017</t>
   </si>
   <si>
     <t>Fraud in the Digital Age</t>
@@ -145,13 +145,13 @@
     <t>Instruction</t>
   </si>
   <si>
-    <t>2017-12-18T18:30:00.000Z</t>
+    <t>12/18/2017</t>
   </si>
   <si>
     <t>Prolaera</t>
   </si>
   <si>
-    <t>2017-02-12T08:00:00.000Z</t>
+    <t>2/12/2017</t>
   </si>
   <si>
     <t>A&amp;A Conference 2017</t>
@@ -163,16 +163,25 @@
     <t>Group-Live</t>
   </si>
   <si>
-    <t>2017-06-14T19:00:00.000Z</t>
+    <t>6/14/2017</t>
   </si>
   <si>
     <t>Federal Tax Updates</t>
   </si>
   <si>
-    <t>2017-09-01T07:00:00.000Z</t>
-  </si>
-  <si>
-    <t>2017-11-01T08:00:00.000Z</t>
+    <t>11/1/2017</t>
+  </si>
+  <si>
+    <t>Total Credits Applied:</t>
+  </si>
+  <si>
+    <t>Total Credits Earned:</t>
+  </si>
+  <si>
+    <t>Continuing Education Requirement:</t>
+  </si>
+  <si>
+    <t>Credits Remaining:</t>
   </si>
 </sst>
 </file>
@@ -569,7 +578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J27"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -654,6 +663,7 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
+      <c r="C8"/>
       <c r="D8" t="s">
         <v>9</v>
       </c>
@@ -686,6 +696,7 @@
       <c r="B10" t="s">
         <v>14</v>
       </c>
+      <c r="C10"/>
       <c r="D10" t="s">
         <v>15</v>
       </c>
@@ -693,176 +704,186 @@
         <v>16</v>
       </c>
       <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
         <v>2</v>
       </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
+      <c r="C11"/>
       <c r="D11" t="s">
         <v>19</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
       </c>
-      <c r="J11">
+      <c r="I11">
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
+      <c r="C12"/>
       <c r="E12" t="s">
         <v>16</v>
       </c>
-      <c r="J12">
+      <c r="I12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
+      <c r="C13"/>
       <c r="E13" t="s">
         <v>24</v>
       </c>
-      <c r="J13">
+      <c r="I13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
       </c>
+      <c r="C14"/>
       <c r="D14" t="s">
         <v>19</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
       </c>
-      <c r="J14">
+      <c r="I14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
       </c>
+      <c r="C15"/>
       <c r="D15" t="s">
         <v>19</v>
       </c>
       <c r="E15" t="s">
         <v>16</v>
       </c>
-      <c r="J15">
+      <c r="I15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
       </c>
+      <c r="C16"/>
       <c r="D16" t="s">
         <v>19</v>
       </c>
       <c r="E16" t="s">
         <v>31</v>
       </c>
-      <c r="J16">
+      <c r="I16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
       </c>
+      <c r="C17"/>
       <c r="D17" t="s">
         <v>33</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
       </c>
-      <c r="J17">
+      <c r="I17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
       </c>
+      <c r="C18"/>
       <c r="D18" t="s">
         <v>36</v>
       </c>
       <c r="E18" t="s">
         <v>37</v>
       </c>
-      <c r="J18">
+      <c r="I18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
       <c r="B19" t="s">
         <v>39</v>
       </c>
+      <c r="C19"/>
       <c r="D19" t="s">
         <v>19</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
       </c>
-      <c r="J19">
+      <c r="I19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
+      <c r="C20"/>
       <c r="E20" t="s">
         <v>31</v>
       </c>
-      <c r="J20">
+      <c r="I20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
         <v>28</v>
@@ -870,21 +891,72 @@
       <c r="E21" t="s">
         <v>24</v>
       </c>
-      <c r="J21">
+      <c r="I21">
         <v>2</v>
       </c>
     </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="I24">
+        <v>41.5</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25">
+        <v>41.5</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26">
+        <v>36</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="26">
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="A3:F5"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="A6:D7"/>
+    <mergeCell ref="B8:C9"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
@@ -892,6 +964,17 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
add worksheet styles and refactor cell merging logic.
</commit_message>
<xml_diff>
--- a/complianceReport.xlsx
+++ b/complianceReport.xlsx
@@ -1,12 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dillontitcomb/Desktop/prolaera-excel/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="User Compliance Report" state="show" r:id="rId4"/>
+    <sheet name="User Compliance Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,11 +41,19 @@
     <r>
       <rPr>
         <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">License #: </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>123123123</t>
     </r>
   </si>
@@ -37,11 +61,19 @@
     <r>
       <rPr>
         <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Issue Date: </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>12/31/2017</t>
     </r>
   </si>
@@ -49,11 +81,19 @@
     <r>
       <rPr>
         <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Reporting Period: </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>12/30/2016 - 12/31/2017</t>
     </r>
   </si>
@@ -61,11 +101,19 @@
     <r>
       <rPr>
         <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
       </rPr>
       <t xml:space="preserve">Cycle Total: </t>
     </r>
     <r>
-      <rPr/>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>12/30/2016 - 12/31/2017</t>
     </r>
   </si>
@@ -187,22 +235,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,20 +286,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,27 +643,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22:I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="J1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -607,96 +681,103 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8"/>
-      <c r="D8" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I8" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C10"/>
+      <c r="C10" s="6"/>
       <c r="D10" t="s">
         <v>15</v>
       </c>
@@ -710,14 +791,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11"/>
+      <c r="C11" s="6"/>
       <c r="D11" t="s">
         <v>19</v>
       </c>
@@ -728,14 +809,14 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12"/>
+      <c r="C12" s="6"/>
       <c r="E12" t="s">
         <v>16</v>
       </c>
@@ -743,14 +824,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C13"/>
+      <c r="C13" s="6"/>
       <c r="E13" t="s">
         <v>24</v>
       </c>
@@ -758,14 +839,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C14"/>
+      <c r="C14" s="6"/>
       <c r="D14" t="s">
         <v>19</v>
       </c>
@@ -776,14 +857,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C15"/>
+      <c r="C15" s="6"/>
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -794,14 +875,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C16"/>
+      <c r="C16" s="6"/>
       <c r="D16" t="s">
         <v>19</v>
       </c>
@@ -812,14 +893,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C17"/>
+      <c r="C17" s="6"/>
       <c r="D17" t="s">
         <v>33</v>
       </c>
@@ -830,14 +911,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C18"/>
+      <c r="C18" s="6"/>
       <c r="D18" t="s">
         <v>36</v>
       </c>
@@ -848,14 +929,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C19"/>
+      <c r="C19" s="6"/>
       <c r="D19" t="s">
         <v>19</v>
       </c>
@@ -866,14 +947,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C20"/>
+      <c r="C20" s="6"/>
       <c r="E20" t="s">
         <v>31</v>
       </c>
@@ -881,7 +962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -895,18 +976,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I22" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>41</v>
       </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
       <c r="I24">
         <v>41.5</v>
       </c>
@@ -914,10 +1020,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
       <c r="I25">
         <v>41.5</v>
       </c>
@@ -925,10 +1036,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>43</v>
       </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
       <c r="I26">
         <v>36</v>
       </c>
@@ -936,10 +1052,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
       <c r="I27">
         <v>0</v>
       </c>
@@ -947,36 +1068,59 @@
         <v>2</v>
       </c>
     </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="A3:F5"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="A6:D7"/>
+  <mergeCells count="40">
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:F28"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A6:F7"/>
     <mergeCell ref="B8:C9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:F5"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add subHeader builder component that takes year or category input and generates the cycle name and period accordingly.
</commit_message>
<xml_diff>
--- a/complianceReport.xlsx
+++ b/complianceReport.xlsx
@@ -5,13 +5,14 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="User Compliance Report" state="show" r:id="rId4"/>
+    <sheet sheetId="2" name="Components Test" state="show" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="94">
   <si>
     <t>Washington CPA</t>
   </si>
@@ -320,6 +321,42 @@
   </si>
   <si>
     <t>Credits Remaining:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Annual Total: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>1/1/2015 - 12/30/2015</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Annual Total: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>1/1/2016 - 12/30/2016</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Annual Total: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>1/1/2017 - 12/30/2017</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1709,4 +1746,176 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J11"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="G1:J2"/>
+    <mergeCell ref="A3:F5"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="A6:J7"/>
+    <mergeCell ref="A8:J9"/>
+    <mergeCell ref="A10:J11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix error with default cycle table body output.
</commit_message>
<xml_diff>
--- a/complianceReport.xlsx
+++ b/complianceReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="91">
   <si>
     <t>Washington CPA</t>
   </si>
@@ -321,42 +321,6 @@
   </si>
   <si>
     <t>Credits Remaining:</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t xml:space="preserve">Annual Total: </t>
-    </r>
-    <r>
-      <rPr/>
-      <t>1/1/2017 - 12/30/2017</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t xml:space="preserve">Non-Tech Total: </t>
-    </r>
-    <r>
-      <rPr/>
-      <t>12/30/2016 - 12/31/2019</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t xml:space="preserve">Technical Total: </t>
-    </r>
-    <r>
-      <rPr/>
-      <t>12/30/2016 - 12/31/2019</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -1750,7 +1714,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J45"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1827,7 +1791,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>91</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2300,94 +2264,99 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" t="s">
+        <v>35</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" t="s">
+        <v>57</v>
+      </c>
+      <c r="I38">
+        <v>4</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="J39">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="D40" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="J40">
         <v>2</v>
@@ -2395,1222 +2364,91 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>26</v>
+      </c>
+      <c r="D41" t="s">
+        <v>46</v>
       </c>
       <c r="E41" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="J41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="E42" t="s">
+        <v>27</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" t="s">
+        <v>83</v>
+      </c>
+      <c r="J43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" t="s">
+        <v>35</v>
+      </c>
+      <c r="J44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" t="s">
         <v>57</v>
       </c>
-      <c r="J42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" t="s">
-        <v>15</v>
-      </c>
-      <c r="D47" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" t="s">
-        <v>17</v>
-      </c>
-      <c r="J47">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" t="s">
-        <v>19</v>
-      </c>
-      <c r="D48" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" t="s">
-        <v>21</v>
-      </c>
-      <c r="J48">
+      <c r="J45">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>22</v>
-      </c>
-      <c r="B49" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" t="s">
-        <v>24</v>
-      </c>
-      <c r="E49" t="s">
-        <v>17</v>
-      </c>
-      <c r="J49">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>28</v>
-      </c>
-      <c r="B50" t="s">
-        <v>29</v>
-      </c>
-      <c r="D50" t="s">
-        <v>30</v>
-      </c>
-      <c r="E50" t="s">
-        <v>27</v>
-      </c>
-      <c r="J50">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>33</v>
-      </c>
-      <c r="B51" t="s">
-        <v>34</v>
-      </c>
-      <c r="D51" t="s">
-        <v>30</v>
-      </c>
-      <c r="E51" t="s">
-        <v>35</v>
-      </c>
-      <c r="J51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>36</v>
-      </c>
-      <c r="B52" t="s">
-        <v>37</v>
-      </c>
-      <c r="E52" t="s">
-        <v>17</v>
-      </c>
-      <c r="J52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>38</v>
-      </c>
-      <c r="B53" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" t="s">
-        <v>27</v>
-      </c>
-      <c r="J53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>33</v>
-      </c>
-      <c r="B54" t="s">
-        <v>39</v>
-      </c>
-      <c r="D54" t="s">
-        <v>30</v>
-      </c>
-      <c r="E54" t="s">
-        <v>35</v>
-      </c>
-      <c r="J54">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>40</v>
-      </c>
-      <c r="B55" t="s">
-        <v>41</v>
-      </c>
-      <c r="D55" t="s">
-        <v>42</v>
-      </c>
-      <c r="E55" t="s">
-        <v>27</v>
-      </c>
-      <c r="J55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>28</v>
-      </c>
-      <c r="B56" t="s">
-        <v>43</v>
-      </c>
-      <c r="D56" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" t="s">
-        <v>27</v>
-      </c>
-      <c r="J56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>40</v>
-      </c>
-      <c r="B57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D57" t="s">
-        <v>30</v>
-      </c>
-      <c r="E57" t="s">
-        <v>35</v>
-      </c>
-      <c r="J57">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>45</v>
-      </c>
-      <c r="B58" t="s">
-        <v>43</v>
-      </c>
-      <c r="D58" t="s">
-        <v>46</v>
-      </c>
-      <c r="E58" t="s">
-        <v>27</v>
-      </c>
-      <c r="J58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>47</v>
-      </c>
-      <c r="B59" t="s">
-        <v>48</v>
-      </c>
-      <c r="E59" t="s">
-        <v>17</v>
-      </c>
-      <c r="J59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>49</v>
-      </c>
-      <c r="B60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E60" t="s">
-        <v>17</v>
-      </c>
-      <c r="J60">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>50</v>
-      </c>
-      <c r="B61" t="s">
-        <v>51</v>
-      </c>
-      <c r="D61" t="s">
-        <v>30</v>
-      </c>
-      <c r="E61" t="s">
-        <v>35</v>
-      </c>
-      <c r="J61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>52</v>
-      </c>
-      <c r="B62" t="s">
-        <v>53</v>
-      </c>
-      <c r="D62" t="s">
-        <v>30</v>
-      </c>
-      <c r="E62" t="s">
-        <v>35</v>
-      </c>
-      <c r="J62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>54</v>
-      </c>
-      <c r="B63" t="s">
-        <v>55</v>
-      </c>
-      <c r="D63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E63" t="s">
-        <v>27</v>
-      </c>
-      <c r="J63">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>56</v>
-      </c>
-      <c r="B64" t="s">
-        <v>55</v>
-      </c>
-      <c r="E64" t="s">
-        <v>57</v>
-      </c>
-      <c r="J64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>58</v>
-      </c>
-      <c r="B65" t="s">
-        <v>59</v>
-      </c>
-      <c r="E65" t="s">
-        <v>57</v>
-      </c>
-      <c r="J65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>60</v>
-      </c>
-      <c r="B66" t="s">
-        <v>61</v>
-      </c>
-      <c r="D66" t="s">
-        <v>20</v>
-      </c>
-      <c r="E66" t="s">
-        <v>27</v>
-      </c>
-      <c r="J66">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>64</v>
-      </c>
-      <c r="B67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" t="s">
-        <v>20</v>
-      </c>
-      <c r="E67" t="s">
-        <v>27</v>
-      </c>
-      <c r="J67">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>18</v>
-      </c>
-      <c r="B68" t="s">
-        <v>19</v>
-      </c>
-      <c r="D68" t="s">
-        <v>42</v>
-      </c>
-      <c r="E68" t="s">
-        <v>21</v>
-      </c>
-      <c r="J68">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" t="s">
-        <v>44</v>
-      </c>
-      <c r="D69" t="s">
-        <v>20</v>
-      </c>
-      <c r="E69" t="s">
-        <v>66</v>
-      </c>
-      <c r="J69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>67</v>
-      </c>
-      <c r="B70" t="s">
-        <v>68</v>
-      </c>
-      <c r="D70" t="s">
-        <v>69</v>
-      </c>
-      <c r="E70" t="s">
-        <v>57</v>
-      </c>
-      <c r="J70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>71</v>
-      </c>
-      <c r="E71" t="s">
-        <v>35</v>
-      </c>
-      <c r="J71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>75</v>
-      </c>
-      <c r="B72" t="s">
-        <v>76</v>
-      </c>
-      <c r="D72" t="s">
-        <v>20</v>
-      </c>
-      <c r="E72" t="s">
-        <v>35</v>
-      </c>
-      <c r="J72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>77</v>
-      </c>
-      <c r="B73" t="s">
-        <v>78</v>
-      </c>
-      <c r="D73" t="s">
-        <v>16</v>
-      </c>
-      <c r="E73" t="s">
-        <v>35</v>
-      </c>
-      <c r="J73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" t="s">
-        <v>26</v>
-      </c>
-      <c r="D74" t="s">
-        <v>46</v>
-      </c>
-      <c r="E74" t="s">
-        <v>35</v>
-      </c>
-      <c r="J74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>80</v>
-      </c>
-      <c r="B75" t="s">
-        <v>29</v>
-      </c>
-      <c r="D75" t="s">
-        <v>16</v>
-      </c>
-      <c r="E75" t="s">
-        <v>27</v>
-      </c>
-      <c r="J75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>80</v>
-      </c>
-      <c r="B76" t="s">
-        <v>81</v>
-      </c>
-      <c r="D76" t="s">
-        <v>82</v>
-      </c>
-      <c r="E76" t="s">
-        <v>83</v>
-      </c>
-      <c r="J76">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>80</v>
-      </c>
-      <c r="B77" t="s">
-        <v>84</v>
-      </c>
-      <c r="D77" t="s">
-        <v>16</v>
-      </c>
-      <c r="E77" t="s">
-        <v>35</v>
-      </c>
-      <c r="J77">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>85</v>
-      </c>
-      <c r="B78" t="s">
-        <v>86</v>
-      </c>
-      <c r="D78" t="s">
-        <v>69</v>
-      </c>
-      <c r="E78" t="s">
-        <v>57</v>
-      </c>
-      <c r="J78">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-      <c r="J79" s="4"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>22</v>
-      </c>
-      <c r="B83" t="s">
-        <v>23</v>
-      </c>
-      <c r="D83" t="s">
-        <v>24</v>
-      </c>
-      <c r="E83" t="s">
-        <v>17</v>
-      </c>
-      <c r="J83">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>25</v>
-      </c>
-      <c r="B84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D84" t="s">
-        <v>20</v>
-      </c>
-      <c r="E84" t="s">
-        <v>27</v>
-      </c>
-      <c r="J84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>62</v>
-      </c>
-      <c r="B85" t="s">
-        <v>63</v>
-      </c>
-      <c r="E85" t="s">
-        <v>57</v>
-      </c>
-      <c r="J85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>72</v>
-      </c>
-      <c r="B86" t="s">
-        <v>73</v>
-      </c>
-      <c r="D86" t="s">
-        <v>74</v>
-      </c>
-      <c r="E86" t="s">
-        <v>57</v>
-      </c>
-      <c r="J86">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-      <c r="J87" s="4"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="4"/>
-      <c r="I88" s="4"/>
-      <c r="J88" s="4"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I89" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J89" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
-      <c r="H90" s="5"/>
-      <c r="I90" s="5"/>
-      <c r="J90" s="5"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>14</v>
-      </c>
-      <c r="B91" t="s">
-        <v>15</v>
-      </c>
-      <c r="D91" t="s">
-        <v>16</v>
-      </c>
-      <c r="E91" t="s">
-        <v>17</v>
-      </c>
-      <c r="J91">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>18</v>
-      </c>
-      <c r="B92" t="s">
-        <v>19</v>
-      </c>
-      <c r="D92" t="s">
-        <v>20</v>
-      </c>
-      <c r="E92" t="s">
-        <v>21</v>
-      </c>
-      <c r="J92">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>22</v>
-      </c>
-      <c r="B93" t="s">
-        <v>23</v>
-      </c>
-      <c r="D93" t="s">
-        <v>24</v>
-      </c>
-      <c r="E93" t="s">
-        <v>17</v>
-      </c>
-      <c r="I93">
-        <v>3</v>
-      </c>
-      <c r="J93">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>25</v>
-      </c>
-      <c r="B94" t="s">
-        <v>26</v>
-      </c>
-      <c r="D94" t="s">
-        <v>20</v>
-      </c>
-      <c r="E94" t="s">
-        <v>27</v>
-      </c>
-      <c r="I94">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>28</v>
-      </c>
-      <c r="B95" t="s">
-        <v>29</v>
-      </c>
-      <c r="D95" t="s">
-        <v>30</v>
-      </c>
-      <c r="E95" t="s">
-        <v>27</v>
-      </c>
-      <c r="J95">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>31</v>
-      </c>
-      <c r="B96" t="s">
-        <v>32</v>
-      </c>
-      <c r="D96" t="s">
-        <v>24</v>
-      </c>
-      <c r="E96" t="s">
-        <v>17</v>
-      </c>
-      <c r="H96">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>33</v>
-      </c>
-      <c r="B97" t="s">
-        <v>34</v>
-      </c>
-      <c r="D97" t="s">
-        <v>30</v>
-      </c>
-      <c r="E97" t="s">
-        <v>35</v>
-      </c>
-      <c r="J97">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>36</v>
-      </c>
-      <c r="B98" t="s">
-        <v>37</v>
-      </c>
-      <c r="E98" t="s">
-        <v>17</v>
-      </c>
-      <c r="J98">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>38</v>
-      </c>
-      <c r="B99" t="s">
-        <v>29</v>
-      </c>
-      <c r="D99" t="s">
-        <v>16</v>
-      </c>
-      <c r="E99" t="s">
-        <v>27</v>
-      </c>
-      <c r="J99">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>33</v>
-      </c>
-      <c r="B100" t="s">
-        <v>39</v>
-      </c>
-      <c r="D100" t="s">
-        <v>30</v>
-      </c>
-      <c r="E100" t="s">
-        <v>35</v>
-      </c>
-      <c r="J100">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>40</v>
-      </c>
-      <c r="B101" t="s">
-        <v>41</v>
-      </c>
-      <c r="D101" t="s">
-        <v>42</v>
-      </c>
-      <c r="E101" t="s">
-        <v>27</v>
-      </c>
-      <c r="J101">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>28</v>
-      </c>
-      <c r="B102" t="s">
-        <v>43</v>
-      </c>
-      <c r="D102" t="s">
-        <v>20</v>
-      </c>
-      <c r="E102" t="s">
-        <v>27</v>
-      </c>
-      <c r="J102">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>40</v>
-      </c>
-      <c r="B103" t="s">
-        <v>44</v>
-      </c>
-      <c r="D103" t="s">
-        <v>30</v>
-      </c>
-      <c r="E103" t="s">
-        <v>35</v>
-      </c>
-      <c r="J103">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>45</v>
-      </c>
-      <c r="B104" t="s">
-        <v>43</v>
-      </c>
-      <c r="D104" t="s">
-        <v>46</v>
-      </c>
-      <c r="E104" t="s">
-        <v>27</v>
-      </c>
-      <c r="J104">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>47</v>
-      </c>
-      <c r="B105" t="s">
-        <v>48</v>
-      </c>
-      <c r="E105" t="s">
-        <v>17</v>
-      </c>
-      <c r="J105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>49</v>
-      </c>
-      <c r="B106" t="s">
-        <v>23</v>
-      </c>
-      <c r="E106" t="s">
-        <v>17</v>
-      </c>
-      <c r="J106">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>50</v>
-      </c>
-      <c r="B107" t="s">
-        <v>51</v>
-      </c>
-      <c r="D107" t="s">
-        <v>30</v>
-      </c>
-      <c r="E107" t="s">
-        <v>35</v>
-      </c>
-      <c r="J107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>52</v>
-      </c>
-      <c r="B108" t="s">
-        <v>53</v>
-      </c>
-      <c r="D108" t="s">
-        <v>30</v>
-      </c>
-      <c r="E108" t="s">
-        <v>35</v>
-      </c>
-      <c r="J108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>54</v>
-      </c>
-      <c r="B109" t="s">
-        <v>55</v>
-      </c>
-      <c r="D109" t="s">
-        <v>20</v>
-      </c>
-      <c r="E109" t="s">
-        <v>27</v>
-      </c>
-      <c r="J109">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>56</v>
-      </c>
-      <c r="B110" t="s">
-        <v>55</v>
-      </c>
-      <c r="E110" t="s">
-        <v>57</v>
-      </c>
-      <c r="J110">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>58</v>
-      </c>
-      <c r="B111" t="s">
-        <v>59</v>
-      </c>
-      <c r="E111" t="s">
-        <v>57</v>
-      </c>
-      <c r="J111">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>60</v>
-      </c>
-      <c r="B112" t="s">
-        <v>61</v>
-      </c>
-      <c r="D112" t="s">
-        <v>20</v>
-      </c>
-      <c r="E112" t="s">
-        <v>27</v>
-      </c>
-      <c r="J112">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>62</v>
-      </c>
-      <c r="B113" t="s">
-        <v>63</v>
-      </c>
-      <c r="E113" t="s">
-        <v>57</v>
-      </c>
-      <c r="I113">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>64</v>
-      </c>
-      <c r="B114" t="s">
-        <v>15</v>
-      </c>
-      <c r="D114" t="s">
-        <v>20</v>
-      </c>
-      <c r="E114" t="s">
-        <v>27</v>
-      </c>
-      <c r="J114">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>18</v>
-      </c>
-      <c r="B115" t="s">
-        <v>19</v>
-      </c>
-      <c r="D115" t="s">
-        <v>42</v>
-      </c>
-      <c r="E115" t="s">
-        <v>21</v>
-      </c>
-      <c r="J115">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="16">
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="G1:J2"/>
     <mergeCell ref="A3:F5"/>
@@ -3627,46 +2465,6 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
-    <mergeCell ref="A35:J36"/>
-    <mergeCell ref="B37:C38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="A43:J44"/>
-    <mergeCell ref="B45:C46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="I45:I46"/>
-    <mergeCell ref="J45:J46"/>
-    <mergeCell ref="A79:J80"/>
-    <mergeCell ref="B81:C82"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="I81:I82"/>
-    <mergeCell ref="J81:J82"/>
-    <mergeCell ref="A87:J88"/>
-    <mergeCell ref="B89:C90"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="H89:H90"/>
-    <mergeCell ref="I89:I90"/>
-    <mergeCell ref="J89:J90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
add table summary builder, add styling to table body and table summary.
</commit_message>
<xml_diff>
--- a/complianceReport.xlsx
+++ b/complianceReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="92">
   <si>
     <t>Washington CPA</t>
   </si>
@@ -321,6 +321,18 @@
   </si>
   <si>
     <t>Credits Remaining:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Non-Tech Total: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>12/30/2016 - 12/31/2019</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1714,7 +1726,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J20"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1791,7 +1803,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1831,14 +1843,10 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1855,600 +1863,168 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C10"/>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
       </c>
       <c r="J10">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C11"/>
       <c r="D11" t="s">
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J11">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C12"/>
       <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="J12">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13">
-        <v>2</v>
+        <v>57</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15">
-        <v>4</v>
-      </c>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" t="s">
-        <v>35</v>
-      </c>
+      <c r="A16" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
       <c r="J16">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" t="s">
-        <v>17</v>
-      </c>
+      <c r="A17" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
       <c r="J17">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18">
-        <v>3</v>
-      </c>
+      <c r="A18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" t="s">
-        <v>35</v>
-      </c>
-      <c r="J19">
-        <v>2</v>
+      <c r="A19" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" t="s">
-        <v>27</v>
-      </c>
-      <c r="J20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-      <c r="J21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" t="s">
-        <v>27</v>
-      </c>
-      <c r="J23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" t="s">
-        <v>35</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" t="s">
-        <v>27</v>
-      </c>
-      <c r="J28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" t="s">
-        <v>55</v>
-      </c>
-      <c r="E29" t="s">
-        <v>57</v>
-      </c>
-      <c r="J29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>58</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" t="s">
-        <v>57</v>
-      </c>
-      <c r="J30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" t="s">
-        <v>27</v>
-      </c>
-      <c r="J31">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" t="s">
-        <v>57</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" t="s">
-        <v>27</v>
-      </c>
-      <c r="J33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" t="s">
-        <v>66</v>
-      </c>
-      <c r="J35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" t="s">
-        <v>57</v>
-      </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" t="s">
-        <v>71</v>
-      </c>
-      <c r="E37" t="s">
-        <v>35</v>
-      </c>
-      <c r="J37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" t="s">
-        <v>74</v>
-      </c>
-      <c r="E38" t="s">
-        <v>57</v>
-      </c>
-      <c r="I38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" t="s">
-        <v>35</v>
-      </c>
-      <c r="J40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D41" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" t="s">
-        <v>35</v>
-      </c>
-      <c r="J41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" t="s">
-        <v>27</v>
-      </c>
-      <c r="J42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" t="s">
-        <v>82</v>
-      </c>
-      <c r="E43" t="s">
-        <v>83</v>
-      </c>
-      <c r="J43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" t="s">
-        <v>35</v>
-      </c>
-      <c r="J44">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E45" t="s">
-        <v>57</v>
-      </c>
-      <c r="J45">
-        <v>3</v>
-      </c>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="32">
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="G1:J2"/>
     <mergeCell ref="A3:F5"/>
@@ -2465,6 +2041,22 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="J8:J9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
break out buildreport component, finish functionality for all report types.
</commit_message>
<xml_diff>
--- a/complianceReport.xlsx
+++ b/complianceReport.xlsx
@@ -5,14 +5,13 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="User Compliance Report" state="show" r:id="rId4"/>
-    <sheet sheetId="2" name="Components Test" state="show" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="97">
   <si>
     <t>Washington CPA</t>
   </si>
@@ -327,7 +326,67 @@
       <rPr>
         <b/>
       </rPr>
+      <t xml:space="preserve">Annual Total: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>1/1/2017 - 12/30/2017</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Annual Total: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>1/1/2018 - 12/30/2018</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Annual Total: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>1/1/2019 - 12/30/2019</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Technical Total: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>12/30/2016 - 12/31/2019</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
       <t xml:space="preserve">Non-Tech Total: </t>
+    </r>
+    <r>
+      <rPr/>
+      <t>12/30/2016 - 12/31/2019</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">Ethics State Total: </t>
     </r>
     <r>
       <rPr/>
@@ -768,7 +827,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J191"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1652,8 +1711,2264 @@
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
     </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57"/>
+      <c r="D57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" t="s">
+        <v>17</v>
+      </c>
+      <c r="J57">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58"/>
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" t="s">
+        <v>21</v>
+      </c>
+      <c r="J58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" t="s">
+        <v>17</v>
+      </c>
+      <c r="I59">
+        <v>3</v>
+      </c>
+      <c r="J59">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60"/>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" t="s">
+        <v>27</v>
+      </c>
+      <c r="I60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" t="s">
+        <v>29</v>
+      </c>
+      <c r="C61"/>
+      <c r="D61" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" t="s">
+        <v>27</v>
+      </c>
+      <c r="J61">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" t="s">
+        <v>17</v>
+      </c>
+      <c r="H62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63"/>
+      <c r="D63" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" t="s">
+        <v>35</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64"/>
+      <c r="E64" t="s">
+        <v>17</v>
+      </c>
+      <c r="J64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65"/>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65" t="s">
+        <v>27</v>
+      </c>
+      <c r="J65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" t="s">
+        <v>39</v>
+      </c>
+      <c r="C66"/>
+      <c r="D66" t="s">
+        <v>30</v>
+      </c>
+      <c r="E66" t="s">
+        <v>35</v>
+      </c>
+      <c r="J66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>40</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67"/>
+      <c r="D67" t="s">
+        <v>42</v>
+      </c>
+      <c r="E67" t="s">
+        <v>27</v>
+      </c>
+      <c r="J67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" t="s">
+        <v>43</v>
+      </c>
+      <c r="C68"/>
+      <c r="D68" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" t="s">
+        <v>27</v>
+      </c>
+      <c r="J68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>40</v>
+      </c>
+      <c r="B69" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69"/>
+      <c r="D69" t="s">
+        <v>30</v>
+      </c>
+      <c r="E69" t="s">
+        <v>35</v>
+      </c>
+      <c r="J69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>45</v>
+      </c>
+      <c r="B70" t="s">
+        <v>43</v>
+      </c>
+      <c r="C70"/>
+      <c r="D70" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70" t="s">
+        <v>27</v>
+      </c>
+      <c r="J70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>47</v>
+      </c>
+      <c r="B71" t="s">
+        <v>48</v>
+      </c>
+      <c r="C71"/>
+      <c r="E71" t="s">
+        <v>17</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" t="s">
+        <v>23</v>
+      </c>
+      <c r="C72"/>
+      <c r="E72" t="s">
+        <v>17</v>
+      </c>
+      <c r="J72">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" t="s">
+        <v>51</v>
+      </c>
+      <c r="C73"/>
+      <c r="D73" t="s">
+        <v>30</v>
+      </c>
+      <c r="E73" t="s">
+        <v>35</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B74" t="s">
+        <v>53</v>
+      </c>
+      <c r="C74"/>
+      <c r="D74" t="s">
+        <v>30</v>
+      </c>
+      <c r="E74" t="s">
+        <v>35</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>54</v>
+      </c>
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75"/>
+      <c r="D75" t="s">
+        <v>20</v>
+      </c>
+      <c r="E75" t="s">
+        <v>27</v>
+      </c>
+      <c r="J75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>56</v>
+      </c>
+      <c r="B76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C76"/>
+      <c r="E76" t="s">
+        <v>57</v>
+      </c>
+      <c r="J76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>58</v>
+      </c>
+      <c r="B77" t="s">
+        <v>59</v>
+      </c>
+      <c r="C77"/>
+      <c r="E77" t="s">
+        <v>57</v>
+      </c>
+      <c r="J77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>60</v>
+      </c>
+      <c r="B78" t="s">
+        <v>61</v>
+      </c>
+      <c r="C78"/>
+      <c r="D78" t="s">
+        <v>20</v>
+      </c>
+      <c r="E78" t="s">
+        <v>27</v>
+      </c>
+      <c r="J78">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B79" t="s">
+        <v>63</v>
+      </c>
+      <c r="C79"/>
+      <c r="E79" t="s">
+        <v>57</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>64</v>
+      </c>
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80"/>
+      <c r="D80" t="s">
+        <v>20</v>
+      </c>
+      <c r="E80" t="s">
+        <v>27</v>
+      </c>
+      <c r="J80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" t="s">
+        <v>42</v>
+      </c>
+      <c r="E81" t="s">
+        <v>21</v>
+      </c>
+      <c r="J81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="6"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I82" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J82" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="H84">
+        <v>4</v>
+      </c>
+      <c r="I84">
+        <v>6</v>
+      </c>
+      <c r="J84">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="H85">
+        <v>4</v>
+      </c>
+      <c r="I85">
+        <v>6</v>
+      </c>
+      <c r="J85">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9">
+        <v>4</v>
+      </c>
+      <c r="I86" s="9"/>
+      <c r="J86" s="9"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11">
+        <v>0</v>
+      </c>
+      <c r="I87" s="11">
+        <v>0</v>
+      </c>
+      <c r="J87" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="10"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="11"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="11"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I91" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>65</v>
+      </c>
+      <c r="B93" t="s">
+        <v>44</v>
+      </c>
+      <c r="C93"/>
+      <c r="D93" t="s">
+        <v>20</v>
+      </c>
+      <c r="E93" t="s">
+        <v>66</v>
+      </c>
+      <c r="J93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>67</v>
+      </c>
+      <c r="B94" t="s">
+        <v>68</v>
+      </c>
+      <c r="C94"/>
+      <c r="D94" t="s">
+        <v>69</v>
+      </c>
+      <c r="E94" t="s">
+        <v>57</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>70</v>
+      </c>
+      <c r="B95" t="s">
+        <v>71</v>
+      </c>
+      <c r="C95"/>
+      <c r="E95" t="s">
+        <v>35</v>
+      </c>
+      <c r="J95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>72</v>
+      </c>
+      <c r="B96" t="s">
+        <v>73</v>
+      </c>
+      <c r="C96"/>
+      <c r="D96" t="s">
+        <v>74</v>
+      </c>
+      <c r="E96" t="s">
+        <v>57</v>
+      </c>
+      <c r="I96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>75</v>
+      </c>
+      <c r="B97" t="s">
+        <v>76</v>
+      </c>
+      <c r="C97"/>
+      <c r="D97" t="s">
+        <v>20</v>
+      </c>
+      <c r="E97" t="s">
+        <v>35</v>
+      </c>
+      <c r="J97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>77</v>
+      </c>
+      <c r="B98" t="s">
+        <v>78</v>
+      </c>
+      <c r="C98"/>
+      <c r="D98" t="s">
+        <v>16</v>
+      </c>
+      <c r="E98" t="s">
+        <v>35</v>
+      </c>
+      <c r="J98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C99"/>
+      <c r="D99" t="s">
+        <v>46</v>
+      </c>
+      <c r="E99" t="s">
+        <v>35</v>
+      </c>
+      <c r="J99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>80</v>
+      </c>
+      <c r="B100" t="s">
+        <v>29</v>
+      </c>
+      <c r="C100"/>
+      <c r="D100" t="s">
+        <v>16</v>
+      </c>
+      <c r="E100" t="s">
+        <v>27</v>
+      </c>
+      <c r="J100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>80</v>
+      </c>
+      <c r="B101" t="s">
+        <v>81</v>
+      </c>
+      <c r="C101"/>
+      <c r="D101" t="s">
+        <v>82</v>
+      </c>
+      <c r="E101" t="s">
+        <v>83</v>
+      </c>
+      <c r="J101">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>80</v>
+      </c>
+      <c r="B102" t="s">
+        <v>84</v>
+      </c>
+      <c r="C102"/>
+      <c r="D102" t="s">
+        <v>16</v>
+      </c>
+      <c r="E102" t="s">
+        <v>35</v>
+      </c>
+      <c r="J102">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>85</v>
+      </c>
+      <c r="B103" t="s">
+        <v>86</v>
+      </c>
+      <c r="D103" t="s">
+        <v>69</v>
+      </c>
+      <c r="E103" t="s">
+        <v>57</v>
+      </c>
+      <c r="J103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="6"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I104" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J104" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="6"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+      <c r="F106" s="7"/>
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106">
+        <v>4</v>
+      </c>
+      <c r="J106">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B107" s="7"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+      <c r="F107" s="7"/>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107">
+        <v>4</v>
+      </c>
+      <c r="J107">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9">
+        <v>4</v>
+      </c>
+      <c r="I108" s="9"/>
+      <c r="J108" s="9"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B109" s="10"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="10"/>
+      <c r="G109" s="11"/>
+      <c r="H109" s="11">
+        <v>4</v>
+      </c>
+      <c r="I109" s="11">
+        <v>0</v>
+      </c>
+      <c r="J109" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="10"/>
+      <c r="B110" s="10"/>
+      <c r="C110" s="10"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10"/>
+      <c r="G110" s="11"/>
+      <c r="H110" s="11"/>
+      <c r="I110" s="11"/>
+      <c r="J110" s="11"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="4"/>
+      <c r="J111" s="4"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="4"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
+      <c r="J112" s="4"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="H113" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I113" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J113" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" s="5"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5"/>
+      <c r="G114" s="5"/>
+      <c r="H114" s="5"/>
+      <c r="I114" s="5"/>
+      <c r="J114" s="5"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" s="6"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I115" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J115" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" s="6"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B117" s="7"/>
+      <c r="C117" s="7"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B118" s="7"/>
+      <c r="C118" s="7"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
+      <c r="F118" s="7"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B119" s="8"/>
+      <c r="C119" s="8"/>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8"/>
+      <c r="F119" s="8"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="9">
+        <v>4</v>
+      </c>
+      <c r="I119" s="9"/>
+      <c r="J119" s="9"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A120" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B120" s="10"/>
+      <c r="C120" s="10"/>
+      <c r="D120" s="10"/>
+      <c r="E120" s="10"/>
+      <c r="F120" s="10"/>
+      <c r="G120" s="11"/>
+      <c r="H120" s="11">
+        <v>0</v>
+      </c>
+      <c r="I120" s="11">
+        <v>0</v>
+      </c>
+      <c r="J120" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A121" s="10"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="10"/>
+      <c r="G121" s="11"/>
+      <c r="H121" s="11"/>
+      <c r="I121" s="11"/>
+      <c r="J121" s="11"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="4"/>
+      <c r="J122" s="4"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+      <c r="H123" s="4"/>
+      <c r="I123" s="4"/>
+      <c r="J123" s="4"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F124" s="5"/>
+      <c r="G124" s="5"/>
+      <c r="H124" s="5"/>
+      <c r="I124" s="5"/>
+      <c r="J124" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A125" s="5"/>
+      <c r="B125" s="5"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="5"/>
+      <c r="G125" s="5"/>
+      <c r="H125" s="5"/>
+      <c r="I125" s="5"/>
+      <c r="J125" s="5"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>14</v>
+      </c>
+      <c r="B126" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126"/>
+      <c r="D126" t="s">
+        <v>16</v>
+      </c>
+      <c r="E126" t="s">
+        <v>17</v>
+      </c>
+      <c r="J126">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>18</v>
+      </c>
+      <c r="B127" t="s">
+        <v>19</v>
+      </c>
+      <c r="C127"/>
+      <c r="D127" t="s">
+        <v>20</v>
+      </c>
+      <c r="E127" t="s">
+        <v>21</v>
+      </c>
+      <c r="J127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>22</v>
+      </c>
+      <c r="B128" t="s">
+        <v>23</v>
+      </c>
+      <c r="C128"/>
+      <c r="D128" t="s">
+        <v>24</v>
+      </c>
+      <c r="E128" t="s">
+        <v>17</v>
+      </c>
+      <c r="J128">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>28</v>
+      </c>
+      <c r="B129" t="s">
+        <v>29</v>
+      </c>
+      <c r="C129"/>
+      <c r="D129" t="s">
+        <v>30</v>
+      </c>
+      <c r="E129" t="s">
+        <v>27</v>
+      </c>
+      <c r="J129">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>33</v>
+      </c>
+      <c r="B130" t="s">
+        <v>34</v>
+      </c>
+      <c r="C130"/>
+      <c r="D130" t="s">
+        <v>30</v>
+      </c>
+      <c r="E130" t="s">
+        <v>35</v>
+      </c>
+      <c r="J130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>36</v>
+      </c>
+      <c r="B131" t="s">
+        <v>37</v>
+      </c>
+      <c r="C131"/>
+      <c r="E131" t="s">
+        <v>17</v>
+      </c>
+      <c r="J131">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>38</v>
+      </c>
+      <c r="B132" t="s">
+        <v>29</v>
+      </c>
+      <c r="C132"/>
+      <c r="D132" t="s">
+        <v>16</v>
+      </c>
+      <c r="E132" t="s">
+        <v>27</v>
+      </c>
+      <c r="J132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>33</v>
+      </c>
+      <c r="B133" t="s">
+        <v>39</v>
+      </c>
+      <c r="C133"/>
+      <c r="D133" t="s">
+        <v>30</v>
+      </c>
+      <c r="E133" t="s">
+        <v>35</v>
+      </c>
+      <c r="J133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>40</v>
+      </c>
+      <c r="B134" t="s">
+        <v>41</v>
+      </c>
+      <c r="C134"/>
+      <c r="D134" t="s">
+        <v>42</v>
+      </c>
+      <c r="E134" t="s">
+        <v>27</v>
+      </c>
+      <c r="J134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>28</v>
+      </c>
+      <c r="B135" t="s">
+        <v>43</v>
+      </c>
+      <c r="C135"/>
+      <c r="D135" t="s">
+        <v>20</v>
+      </c>
+      <c r="E135" t="s">
+        <v>27</v>
+      </c>
+      <c r="J135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>40</v>
+      </c>
+      <c r="B136" t="s">
+        <v>44</v>
+      </c>
+      <c r="C136"/>
+      <c r="D136" t="s">
+        <v>30</v>
+      </c>
+      <c r="E136" t="s">
+        <v>35</v>
+      </c>
+      <c r="J136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>45</v>
+      </c>
+      <c r="B137" t="s">
+        <v>43</v>
+      </c>
+      <c r="C137"/>
+      <c r="D137" t="s">
+        <v>46</v>
+      </c>
+      <c r="E137" t="s">
+        <v>27</v>
+      </c>
+      <c r="J137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>47</v>
+      </c>
+      <c r="B138" t="s">
+        <v>48</v>
+      </c>
+      <c r="C138"/>
+      <c r="E138" t="s">
+        <v>17</v>
+      </c>
+      <c r="J138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>49</v>
+      </c>
+      <c r="B139" t="s">
+        <v>23</v>
+      </c>
+      <c r="C139"/>
+      <c r="E139" t="s">
+        <v>17</v>
+      </c>
+      <c r="J139">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>50</v>
+      </c>
+      <c r="B140" t="s">
+        <v>51</v>
+      </c>
+      <c r="C140"/>
+      <c r="D140" t="s">
+        <v>30</v>
+      </c>
+      <c r="E140" t="s">
+        <v>35</v>
+      </c>
+      <c r="J140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>52</v>
+      </c>
+      <c r="B141" t="s">
+        <v>53</v>
+      </c>
+      <c r="C141"/>
+      <c r="D141" t="s">
+        <v>30</v>
+      </c>
+      <c r="E141" t="s">
+        <v>35</v>
+      </c>
+      <c r="J141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>54</v>
+      </c>
+      <c r="B142" t="s">
+        <v>55</v>
+      </c>
+      <c r="C142"/>
+      <c r="D142" t="s">
+        <v>20</v>
+      </c>
+      <c r="E142" t="s">
+        <v>27</v>
+      </c>
+      <c r="J142">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>56</v>
+      </c>
+      <c r="B143" t="s">
+        <v>55</v>
+      </c>
+      <c r="C143"/>
+      <c r="E143" t="s">
+        <v>57</v>
+      </c>
+      <c r="J143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>58</v>
+      </c>
+      <c r="B144" t="s">
+        <v>59</v>
+      </c>
+      <c r="C144"/>
+      <c r="E144" t="s">
+        <v>57</v>
+      </c>
+      <c r="J144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>60</v>
+      </c>
+      <c r="B145" t="s">
+        <v>61</v>
+      </c>
+      <c r="C145"/>
+      <c r="D145" t="s">
+        <v>20</v>
+      </c>
+      <c r="E145" t="s">
+        <v>27</v>
+      </c>
+      <c r="J145">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>64</v>
+      </c>
+      <c r="B146" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146"/>
+      <c r="D146" t="s">
+        <v>20</v>
+      </c>
+      <c r="E146" t="s">
+        <v>27</v>
+      </c>
+      <c r="J146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>18</v>
+      </c>
+      <c r="B147" t="s">
+        <v>19</v>
+      </c>
+      <c r="C147"/>
+      <c r="D147" t="s">
+        <v>42</v>
+      </c>
+      <c r="E147" t="s">
+        <v>21</v>
+      </c>
+      <c r="J147">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>65</v>
+      </c>
+      <c r="B148" t="s">
+        <v>44</v>
+      </c>
+      <c r="C148"/>
+      <c r="D148" t="s">
+        <v>20</v>
+      </c>
+      <c r="E148" t="s">
+        <v>66</v>
+      </c>
+      <c r="J148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>67</v>
+      </c>
+      <c r="B149" t="s">
+        <v>68</v>
+      </c>
+      <c r="C149"/>
+      <c r="D149" t="s">
+        <v>69</v>
+      </c>
+      <c r="E149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>70</v>
+      </c>
+      <c r="B150" t="s">
+        <v>71</v>
+      </c>
+      <c r="C150"/>
+      <c r="E150" t="s">
+        <v>35</v>
+      </c>
+      <c r="J150">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>75</v>
+      </c>
+      <c r="B151" t="s">
+        <v>76</v>
+      </c>
+      <c r="C151"/>
+      <c r="D151" t="s">
+        <v>20</v>
+      </c>
+      <c r="E151" t="s">
+        <v>35</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>77</v>
+      </c>
+      <c r="B152" t="s">
+        <v>78</v>
+      </c>
+      <c r="C152"/>
+      <c r="D152" t="s">
+        <v>16</v>
+      </c>
+      <c r="E152" t="s">
+        <v>35</v>
+      </c>
+      <c r="J152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>79</v>
+      </c>
+      <c r="B153" t="s">
+        <v>26</v>
+      </c>
+      <c r="C153"/>
+      <c r="D153" t="s">
+        <v>46</v>
+      </c>
+      <c r="E153" t="s">
+        <v>35</v>
+      </c>
+      <c r="J153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>80</v>
+      </c>
+      <c r="B154" t="s">
+        <v>29</v>
+      </c>
+      <c r="C154"/>
+      <c r="D154" t="s">
+        <v>16</v>
+      </c>
+      <c r="E154" t="s">
+        <v>27</v>
+      </c>
+      <c r="J154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>80</v>
+      </c>
+      <c r="B155" t="s">
+        <v>81</v>
+      </c>
+      <c r="C155"/>
+      <c r="D155" t="s">
+        <v>82</v>
+      </c>
+      <c r="E155" t="s">
+        <v>83</v>
+      </c>
+      <c r="J155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>80</v>
+      </c>
+      <c r="B156" t="s">
+        <v>84</v>
+      </c>
+      <c r="C156"/>
+      <c r="D156" t="s">
+        <v>16</v>
+      </c>
+      <c r="E156" t="s">
+        <v>35</v>
+      </c>
+      <c r="J156">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>85</v>
+      </c>
+      <c r="B157" t="s">
+        <v>86</v>
+      </c>
+      <c r="D157" t="s">
+        <v>69</v>
+      </c>
+      <c r="E157" t="s">
+        <v>57</v>
+      </c>
+      <c r="J157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158" s="6"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+      <c r="E158" s="6"/>
+      <c r="F158" s="6"/>
+      <c r="G158" s="6"/>
+      <c r="H158" s="6"/>
+      <c r="I158" s="6"/>
+      <c r="J158" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" s="6"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="6"/>
+      <c r="E159" s="6"/>
+      <c r="F159" s="6"/>
+      <c r="G159" s="6"/>
+      <c r="H159" s="6"/>
+      <c r="I159" s="6"/>
+      <c r="J159" s="6"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B160" s="7"/>
+      <c r="C160" s="7"/>
+      <c r="D160" s="7"/>
+      <c r="E160" s="7"/>
+      <c r="F160" s="7"/>
+      <c r="J160">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B161" s="7"/>
+      <c r="C161" s="7"/>
+      <c r="D161" s="7"/>
+      <c r="E161" s="7"/>
+      <c r="F161" s="7"/>
+      <c r="J161">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B162" s="8"/>
+      <c r="C162" s="8"/>
+      <c r="D162" s="8"/>
+      <c r="E162" s="8"/>
+      <c r="F162" s="8"/>
+      <c r="G162" s="9"/>
+      <c r="H162" s="9"/>
+      <c r="I162" s="9"/>
+      <c r="J162" s="9"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B163" s="10"/>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
+      <c r="F163" s="10"/>
+      <c r="G163" s="11"/>
+      <c r="H163" s="11"/>
+      <c r="I163" s="11"/>
+      <c r="J163" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" s="10"/>
+      <c r="B164" s="10"/>
+      <c r="C164" s="10"/>
+      <c r="D164" s="10"/>
+      <c r="E164" s="10"/>
+      <c r="F164" s="10"/>
+      <c r="G164" s="11"/>
+      <c r="H164" s="11"/>
+      <c r="I164" s="11"/>
+      <c r="J164" s="11"/>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B165" s="4"/>
+      <c r="C165" s="4"/>
+      <c r="D165" s="4"/>
+      <c r="E165" s="4"/>
+      <c r="F165" s="4"/>
+      <c r="G165" s="4"/>
+      <c r="H165" s="4"/>
+      <c r="I165" s="4"/>
+      <c r="J165" s="4"/>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A166" s="4"/>
+      <c r="B166" s="4"/>
+      <c r="C166" s="4"/>
+      <c r="D166" s="4"/>
+      <c r="E166" s="4"/>
+      <c r="F166" s="4"/>
+      <c r="G166" s="4"/>
+      <c r="H166" s="4"/>
+      <c r="I166" s="4"/>
+      <c r="J166" s="4"/>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E167" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F167" s="5"/>
+      <c r="G167" s="5"/>
+      <c r="H167" s="5"/>
+      <c r="I167" s="5"/>
+      <c r="J167" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168" s="5"/>
+      <c r="B168" s="5"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="5"/>
+      <c r="E168" s="5"/>
+      <c r="F168" s="5"/>
+      <c r="G168" s="5"/>
+      <c r="H168" s="5"/>
+      <c r="I168" s="5"/>
+      <c r="J168" s="5"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>22</v>
+      </c>
+      <c r="B169" t="s">
+        <v>23</v>
+      </c>
+      <c r="C169"/>
+      <c r="D169" t="s">
+        <v>24</v>
+      </c>
+      <c r="E169" t="s">
+        <v>17</v>
+      </c>
+      <c r="J169">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>25</v>
+      </c>
+      <c r="B170" t="s">
+        <v>26</v>
+      </c>
+      <c r="C170"/>
+      <c r="D170" t="s">
+        <v>20</v>
+      </c>
+      <c r="E170" t="s">
+        <v>27</v>
+      </c>
+      <c r="J170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>62</v>
+      </c>
+      <c r="B171" t="s">
+        <v>63</v>
+      </c>
+      <c r="C171"/>
+      <c r="E171" t="s">
+        <v>57</v>
+      </c>
+      <c r="J171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>72</v>
+      </c>
+      <c r="B172" t="s">
+        <v>73</v>
+      </c>
+      <c r="D172" t="s">
+        <v>74</v>
+      </c>
+      <c r="E172" t="s">
+        <v>57</v>
+      </c>
+      <c r="J172">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173" s="6"/>
+      <c r="B173" s="6"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="6"/>
+      <c r="E173" s="6"/>
+      <c r="F173" s="6"/>
+      <c r="G173" s="6"/>
+      <c r="H173" s="6"/>
+      <c r="I173" s="6"/>
+      <c r="J173" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174" s="6"/>
+      <c r="B174" s="6"/>
+      <c r="C174" s="6"/>
+      <c r="D174" s="6"/>
+      <c r="E174" s="6"/>
+      <c r="F174" s="6"/>
+      <c r="G174" s="6"/>
+      <c r="H174" s="6"/>
+      <c r="I174" s="6"/>
+      <c r="J174" s="6"/>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B175" s="7"/>
+      <c r="C175" s="7"/>
+      <c r="D175" s="7"/>
+      <c r="E175" s="7"/>
+      <c r="F175" s="7"/>
+      <c r="J175">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B176" s="7"/>
+      <c r="C176" s="7"/>
+      <c r="D176" s="7"/>
+      <c r="E176" s="7"/>
+      <c r="F176" s="7"/>
+      <c r="J176">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B177" s="8"/>
+      <c r="C177" s="8"/>
+      <c r="D177" s="8"/>
+      <c r="E177" s="8"/>
+      <c r="F177" s="8"/>
+      <c r="G177" s="9"/>
+      <c r="H177" s="9"/>
+      <c r="I177" s="9"/>
+      <c r="J177" s="9"/>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B178" s="10"/>
+      <c r="C178" s="10"/>
+      <c r="D178" s="10"/>
+      <c r="E178" s="10"/>
+      <c r="F178" s="10"/>
+      <c r="G178" s="11"/>
+      <c r="H178" s="11"/>
+      <c r="I178" s="11"/>
+      <c r="J178" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" s="10"/>
+      <c r="B179" s="10"/>
+      <c r="C179" s="10"/>
+      <c r="D179" s="10"/>
+      <c r="E179" s="10"/>
+      <c r="F179" s="10"/>
+      <c r="G179" s="11"/>
+      <c r="H179" s="11"/>
+      <c r="I179" s="11"/>
+      <c r="J179" s="11"/>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B180" s="4"/>
+      <c r="C180" s="4"/>
+      <c r="D180" s="4"/>
+      <c r="E180" s="4"/>
+      <c r="F180" s="4"/>
+      <c r="G180" s="4"/>
+      <c r="H180" s="4"/>
+      <c r="I180" s="4"/>
+      <c r="J180" s="4"/>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181" s="4"/>
+      <c r="B181" s="4"/>
+      <c r="C181" s="4"/>
+      <c r="D181" s="4"/>
+      <c r="E181" s="4"/>
+      <c r="F181" s="4"/>
+      <c r="G181" s="4"/>
+      <c r="H181" s="4"/>
+      <c r="I181" s="4"/>
+      <c r="J181" s="4"/>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C182" s="5"/>
+      <c r="D182" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E182" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F182" s="5"/>
+      <c r="G182" s="5"/>
+      <c r="H182" s="5"/>
+      <c r="I182" s="5"/>
+      <c r="J182" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" s="5"/>
+      <c r="B183" s="5"/>
+      <c r="C183" s="5"/>
+      <c r="D183" s="5"/>
+      <c r="E183" s="5"/>
+      <c r="F183" s="5"/>
+      <c r="G183" s="5"/>
+      <c r="H183" s="5"/>
+      <c r="I183" s="5"/>
+      <c r="J183" s="5"/>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>31</v>
+      </c>
+      <c r="B184" t="s">
+        <v>32</v>
+      </c>
+      <c r="D184" t="s">
+        <v>24</v>
+      </c>
+      <c r="E184" t="s">
+        <v>17</v>
+      </c>
+      <c r="J184">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185" s="6"/>
+      <c r="B185" s="6"/>
+      <c r="C185" s="6"/>
+      <c r="D185" s="6"/>
+      <c r="E185" s="6"/>
+      <c r="F185" s="6"/>
+      <c r="G185" s="6"/>
+      <c r="H185" s="6"/>
+      <c r="I185" s="6"/>
+      <c r="J185" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186" s="6"/>
+      <c r="B186" s="6"/>
+      <c r="C186" s="6"/>
+      <c r="D186" s="6"/>
+      <c r="E186" s="6"/>
+      <c r="F186" s="6"/>
+      <c r="G186" s="6"/>
+      <c r="H186" s="6"/>
+      <c r="I186" s="6"/>
+      <c r="J186" s="6"/>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B187" s="7"/>
+      <c r="C187" s="7"/>
+      <c r="D187" s="7"/>
+      <c r="E187" s="7"/>
+      <c r="F187" s="7"/>
+      <c r="J187">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B188" s="7"/>
+      <c r="C188" s="7"/>
+      <c r="D188" s="7"/>
+      <c r="E188" s="7"/>
+      <c r="F188" s="7"/>
+      <c r="J188">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B189" s="8"/>
+      <c r="C189" s="8"/>
+      <c r="D189" s="8"/>
+      <c r="E189" s="8"/>
+      <c r="F189" s="8"/>
+      <c r="G189" s="9"/>
+      <c r="H189" s="9"/>
+      <c r="I189" s="9"/>
+      <c r="J189" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B190" s="10"/>
+      <c r="C190" s="10"/>
+      <c r="D190" s="10"/>
+      <c r="E190" s="10"/>
+      <c r="F190" s="10"/>
+      <c r="G190" s="11"/>
+      <c r="H190" s="11"/>
+      <c r="I190" s="11"/>
+      <c r="J190" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191" s="10"/>
+      <c r="B191" s="10"/>
+      <c r="C191" s="10"/>
+      <c r="D191" s="10"/>
+      <c r="E191" s="10"/>
+      <c r="F191" s="10"/>
+      <c r="G191" s="11"/>
+      <c r="H191" s="11"/>
+      <c r="I191" s="11"/>
+      <c r="J191" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="270">
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="G1:J2"/>
     <mergeCell ref="A3:F5"/>
@@ -1718,347 +4033,214 @@
     <mergeCell ref="H51:H52"/>
     <mergeCell ref="I51:I52"/>
     <mergeCell ref="J51:J52"/>
+    <mergeCell ref="A53:J54"/>
+    <mergeCell ref="B55:C56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="J55:J56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="A82:F83"/>
+    <mergeCell ref="G82:G83"/>
+    <mergeCell ref="H82:H83"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="J82:J83"/>
+    <mergeCell ref="A84:F84"/>
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="A86:F86"/>
+    <mergeCell ref="A87:F88"/>
+    <mergeCell ref="G87:G88"/>
+    <mergeCell ref="H87:H88"/>
+    <mergeCell ref="I87:I88"/>
+    <mergeCell ref="J87:J88"/>
+    <mergeCell ref="A89:J90"/>
+    <mergeCell ref="B91:C92"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="H91:H92"/>
+    <mergeCell ref="I91:I92"/>
+    <mergeCell ref="J91:J92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="A104:F105"/>
+    <mergeCell ref="G104:G105"/>
+    <mergeCell ref="H104:H105"/>
+    <mergeCell ref="I104:I105"/>
+    <mergeCell ref="J104:J105"/>
+    <mergeCell ref="A106:F106"/>
+    <mergeCell ref="A107:F107"/>
+    <mergeCell ref="A108:F108"/>
+    <mergeCell ref="A109:F110"/>
+    <mergeCell ref="G109:G110"/>
+    <mergeCell ref="H109:H110"/>
+    <mergeCell ref="I109:I110"/>
+    <mergeCell ref="J109:J110"/>
+    <mergeCell ref="A111:J112"/>
+    <mergeCell ref="B113:C114"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="E113:E114"/>
+    <mergeCell ref="F113:F114"/>
+    <mergeCell ref="G113:G114"/>
+    <mergeCell ref="H113:H114"/>
+    <mergeCell ref="I113:I114"/>
+    <mergeCell ref="J113:J114"/>
+    <mergeCell ref="A115:F116"/>
+    <mergeCell ref="G115:G116"/>
+    <mergeCell ref="H115:H116"/>
+    <mergeCell ref="I115:I116"/>
+    <mergeCell ref="J115:J116"/>
+    <mergeCell ref="A117:F117"/>
+    <mergeCell ref="A118:F118"/>
+    <mergeCell ref="A119:F119"/>
+    <mergeCell ref="A120:F121"/>
+    <mergeCell ref="G120:G121"/>
+    <mergeCell ref="H120:H121"/>
+    <mergeCell ref="I120:I121"/>
+    <mergeCell ref="J120:J121"/>
+    <mergeCell ref="A122:J123"/>
+    <mergeCell ref="B124:C125"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="D124:D125"/>
+    <mergeCell ref="E124:E125"/>
+    <mergeCell ref="F124:F125"/>
+    <mergeCell ref="G124:G125"/>
+    <mergeCell ref="H124:H125"/>
+    <mergeCell ref="I124:I125"/>
+    <mergeCell ref="J124:J125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="A158:F159"/>
+    <mergeCell ref="G158:G159"/>
+    <mergeCell ref="H158:H159"/>
+    <mergeCell ref="I158:I159"/>
+    <mergeCell ref="J158:J159"/>
+    <mergeCell ref="A160:F160"/>
+    <mergeCell ref="A161:F161"/>
+    <mergeCell ref="A162:F162"/>
+    <mergeCell ref="A163:F164"/>
+    <mergeCell ref="G163:G164"/>
+    <mergeCell ref="H163:H164"/>
+    <mergeCell ref="I163:I164"/>
+    <mergeCell ref="J163:J164"/>
+    <mergeCell ref="A165:J166"/>
+    <mergeCell ref="B167:C168"/>
+    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="D167:D168"/>
+    <mergeCell ref="E167:E168"/>
+    <mergeCell ref="F167:F168"/>
+    <mergeCell ref="G167:G168"/>
+    <mergeCell ref="H167:H168"/>
+    <mergeCell ref="I167:I168"/>
+    <mergeCell ref="J167:J168"/>
+    <mergeCell ref="B169:C169"/>
+    <mergeCell ref="B170:C170"/>
+    <mergeCell ref="B171:C171"/>
+    <mergeCell ref="A173:F174"/>
+    <mergeCell ref="G173:G174"/>
+    <mergeCell ref="H173:H174"/>
+    <mergeCell ref="I173:I174"/>
+    <mergeCell ref="J173:J174"/>
+    <mergeCell ref="A175:F175"/>
+    <mergeCell ref="A176:F176"/>
+    <mergeCell ref="A177:F177"/>
+    <mergeCell ref="A178:F179"/>
+    <mergeCell ref="G178:G179"/>
+    <mergeCell ref="H178:H179"/>
+    <mergeCell ref="I178:I179"/>
+    <mergeCell ref="J178:J179"/>
+    <mergeCell ref="A180:J181"/>
+    <mergeCell ref="B182:C183"/>
+    <mergeCell ref="A182:A183"/>
+    <mergeCell ref="D182:D183"/>
+    <mergeCell ref="E182:E183"/>
+    <mergeCell ref="F182:F183"/>
+    <mergeCell ref="G182:G183"/>
+    <mergeCell ref="H182:H183"/>
+    <mergeCell ref="I182:I183"/>
+    <mergeCell ref="J182:J183"/>
+    <mergeCell ref="A185:F186"/>
+    <mergeCell ref="G185:G186"/>
+    <mergeCell ref="H185:H186"/>
+    <mergeCell ref="I185:I186"/>
+    <mergeCell ref="J185:J186"/>
+    <mergeCell ref="A187:F187"/>
+    <mergeCell ref="A188:F188"/>
+    <mergeCell ref="A189:F189"/>
+    <mergeCell ref="A190:F191"/>
+    <mergeCell ref="G190:G191"/>
+    <mergeCell ref="H190:H191"/>
+    <mergeCell ref="I190:I191"/>
+    <mergeCell ref="J190:J191"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10"/>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11"/>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12"/>
-      <c r="E12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="J16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="J17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="G1:J2"/>
-    <mergeCell ref="A3:F5"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="A6:J7"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
 </file>
</xml_diff>